<commit_message>
Updated the python script to load the properly
</commit_message>
<xml_diff>
--- a/dataset/Doctor.xlsx
+++ b/dataset/Doctor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faisa\OneDrive\Documents\Hospital_CAI\Source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shipr\OneDrive\Documents\project\hospital-performance-dashboard\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F28D2B1-0F98-403A-A8F9-824EDF010F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8490402C-4FFC-417E-B2A5-443E3FD78EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{90F7F0BD-DE89-4433-B1CF-7611AB4BAB1F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{90F7F0BD-DE89-4433-B1CF-7611AB4BAB1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="149">
   <si>
     <t>name</t>
   </si>
@@ -59,12 +57,6 @@
     <t>7654321098</t>
   </si>
   <si>
-    <t>6543210987</t>
-  </si>
-  <si>
-    <t>3210987654</t>
-  </si>
-  <si>
     <t>8765432119</t>
   </si>
   <si>
@@ -251,9 +243,6 @@
     <t>7</t>
   </si>
   <si>
-    <t>anita.patel@hospital.com</t>
-  </si>
-  <si>
     <t>D007</t>
   </si>
   <si>
@@ -341,9 +330,6 @@
     <t>2017-08-15</t>
   </si>
   <si>
-    <t>meera.reddy@hospital.com</t>
-  </si>
-  <si>
     <t>D011</t>
   </si>
   <si>
@@ -489,16 +475,30 @@
   </si>
   <si>
     <t>https://i.ibb.co/5g6N8dwD/DR-1.jpg</t>
+  </si>
+  <si>
+    <t>anita.patel12@gmail.com</t>
+  </si>
+  <si>
+    <t>merra.reddy@hospital.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -521,13 +521,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -862,50 +865,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0634226B-9DC8-458C-AF1B-610DAAC1D7F2}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" customWidth="1"/>
-    <col min="9" max="9" width="22.77734375" customWidth="1"/>
-    <col min="10" max="10" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" customWidth="1"/>
+    <col min="9" max="9" width="22.81640625" customWidth="1"/>
+    <col min="10" max="10" width="8.81640625" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
       </c>
       <c r="K1" t="s">
         <v>1</v>
@@ -914,607 +918,634 @@
         <v>2</v>
       </c>
       <c r="M1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" t="s">
         <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
       </c>
       <c r="K2" t="s">
         <v>4</v>
       </c>
       <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="M2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" t="s">
         <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" t="s">
-        <v>134</v>
-      </c>
-      <c r="J3" t="s">
-        <v>37</v>
       </c>
       <c r="K3" t="s">
         <v>5</v>
       </c>
       <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="M3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>41</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>43</v>
       </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
+        <v>131</v>
+      </c>
+      <c r="J4" t="s">
         <v>44</v>
-      </c>
-      <c r="H4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" t="s">
-        <v>135</v>
-      </c>
-      <c r="J4" t="s">
-        <v>46</v>
       </c>
       <c r="K4" t="s">
         <v>6</v>
       </c>
       <c r="L4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="M4" t="s">
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5">
+        <v>6543210987</v>
+      </c>
+      <c r="L5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="1">
+        <v>3448688899</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" t="s">
+        <v>134</v>
+      </c>
+      <c r="J7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7">
+        <v>6734567912</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="M7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" t="s">
+        <v>130</v>
+      </c>
+      <c r="J8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8">
+        <v>3210987654</v>
+      </c>
+      <c r="L8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J9" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9">
+        <v>3678987789</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" t="s">
+        <v>136</v>
+      </c>
+      <c r="J10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10">
+        <v>4679378788</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" t="s">
+        <v>137</v>
+      </c>
+      <c r="J11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11">
+        <v>5878729001</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="M11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" t="s">
+        <v>131</v>
+      </c>
+      <c r="J12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" t="s">
+        <v>103</v>
+      </c>
+      <c r="M12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" t="s">
+        <v>130</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" t="s">
+        <v>109</v>
+      </c>
+      <c r="M13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" t="s">
         <v>50</v>
       </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
+        <v>120</v>
+      </c>
+      <c r="I15" t="s">
+        <v>138</v>
+      </c>
+      <c r="J15" t="s">
         <v>52</v>
       </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J5" t="s">
-        <v>54</v>
-      </c>
-      <c r="K5" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" t="s">
-        <v>147</v>
+      <c r="K15">
+        <v>4579929979</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M15" t="s">
+        <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" t="s">
-        <v>137</v>
-      </c>
-      <c r="J6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K6" t="s">
-        <v>63</v>
-      </c>
-      <c r="M6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" t="s">
-        <v>138</v>
-      </c>
-      <c r="J7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" t="s">
-        <v>77</v>
-      </c>
-      <c r="I8" t="s">
-        <v>134</v>
-      </c>
-      <c r="J8" t="s">
-        <v>78</v>
-      </c>
-      <c r="K8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" t="s">
-        <v>79</v>
-      </c>
-      <c r="M8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I9" t="s">
-        <v>139</v>
-      </c>
-      <c r="J9" t="s">
-        <v>86</v>
-      </c>
-      <c r="K9" t="s">
-        <v>87</v>
-      </c>
-      <c r="M9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" t="s">
-        <v>93</v>
-      </c>
-      <c r="I10" t="s">
-        <v>140</v>
-      </c>
-      <c r="J10" t="s">
-        <v>94</v>
-      </c>
-      <c r="K10" t="s">
-        <v>95</v>
-      </c>
-      <c r="M10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" t="s">
-        <v>100</v>
-      </c>
-      <c r="I11" t="s">
-        <v>141</v>
-      </c>
-      <c r="J11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K11" t="s">
-        <v>101</v>
-      </c>
-      <c r="M11" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>127</v>
+      </c>
+      <c r="I16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J16" t="s">
+        <v>128</v>
+      </c>
+      <c r="K16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" t="s">
+        <v>129</v>
+      </c>
+      <c r="M16" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" t="s">
-        <v>105</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" t="s">
-        <v>106</v>
-      </c>
-      <c r="I12" t="s">
-        <v>135</v>
-      </c>
-      <c r="J12" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" t="s">
-        <v>107</v>
-      </c>
-      <c r="M12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" t="s">
-        <v>112</v>
-      </c>
-      <c r="I13" t="s">
-        <v>134</v>
-      </c>
-      <c r="J13" t="s">
-        <v>37</v>
-      </c>
-      <c r="K13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L13" t="s">
-        <v>113</v>
-      </c>
-      <c r="M13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>114</v>
-      </c>
-      <c r="B14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D14" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" t="s">
-        <v>118</v>
-      </c>
-      <c r="I14" t="s">
-        <v>134</v>
-      </c>
-      <c r="J14" t="s">
-        <v>29</v>
-      </c>
-      <c r="K14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L14" t="s">
-        <v>119</v>
-      </c>
-      <c r="M14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D15" t="s">
-        <v>123</v>
-      </c>
-      <c r="E15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" t="s">
-        <v>124</v>
-      </c>
-      <c r="I15" t="s">
-        <v>142</v>
-      </c>
-      <c r="J15" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" t="s">
-        <v>125</v>
-      </c>
-      <c r="M15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" t="s">
-        <v>128</v>
-      </c>
-      <c r="D16" t="s">
-        <v>129</v>
-      </c>
-      <c r="E16" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" t="s">
-        <v>131</v>
-      </c>
-      <c r="I16" t="s">
-        <v>134</v>
-      </c>
-      <c r="J16" t="s">
-        <v>132</v>
-      </c>
-      <c r="K16" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16" t="s">
-        <v>133</v>
-      </c>
-      <c r="M16" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L7" r:id="rId1" xr:uid="{21CCCEBE-3C16-424C-8BC2-BA25214D9D62}"/>
+    <hyperlink ref="L11" r:id="rId2" xr:uid="{6E7A5660-2510-4499-AC2C-4035FD091543}"/>
+    <hyperlink ref="L15" r:id="rId3" xr:uid="{EDCC297B-400E-4906-8AE7-97D1D824B776}"/>
+    <hyperlink ref="L10" r:id="rId4" xr:uid="{2CF48093-8676-4031-8B97-BB4A74BAA2CD}"/>
+    <hyperlink ref="L14" r:id="rId5" xr:uid="{BF4320B0-5DDB-45E7-AC71-892A8352F468}"/>
+    <hyperlink ref="L9" r:id="rId6" xr:uid="{F027CB5A-AEAF-4E3A-B1AA-38C2995CCA8B}"/>
+    <hyperlink ref="L6" r:id="rId7" xr:uid="{E5811CD0-3849-4FE0-9FF5-AACB23214DB8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>